<commit_message>
added info to notification
</commit_message>
<xml_diff>
--- a/ExcelBugs.xlsx
+++ b/ExcelBugs.xlsx
@@ -56,10 +56,31 @@
     <t>a.1.1</t>
   </si>
   <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>PopesI</t>
+  </si>
+  <si>
+    <t>IN_PROGRESS</t>
+  </si>
+  <si>
+    <t>BUG_STATUS_UPDATED</t>
+  </si>
+  <si>
+    <t>Title 2</t>
+  </si>
+  <si>
+    <t>Description 2</t>
+  </si>
+  <si>
+    <t>a.1.2</t>
+  </si>
+  <si>
     <t>LOW</t>
   </si>
   <si>
-    <t>PopesI</t>
+    <t>PopesII</t>
   </si>
   <si>
     <t>Nobody</t>
@@ -68,27 +89,6 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>BUG_STATUS_UPDATED</t>
-  </si>
-  <si>
-    <t>Title 2</t>
-  </si>
-  <si>
-    <t>Description 2</t>
-  </si>
-  <si>
-    <t>a.1.2</t>
-  </si>
-  <si>
-    <t>CRITICAL</t>
-  </si>
-  <si>
-    <t>PopesII</t>
-  </si>
-  <si>
-    <t>IN_PROGRESS</t>
-  </si>
-  <si>
     <t>Title 3</t>
   </si>
   <si>
@@ -98,57 +98,57 @@
     <t>a.1.3</t>
   </si>
   <si>
+    <t>PopesIII</t>
+  </si>
+  <si>
+    <t>Title 4</t>
+  </si>
+  <si>
+    <t>Description 4</t>
+  </si>
+  <si>
+    <t>a.1.4</t>
+  </si>
+  <si>
+    <t>PopesIIn</t>
+  </si>
+  <si>
+    <t>Title 5</t>
+  </si>
+  <si>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>a.1.5</t>
+  </si>
+  <si>
     <t>PopesIn</t>
   </si>
   <si>
-    <t>Title 4</t>
-  </si>
-  <si>
-    <t>Description 4</t>
-  </si>
-  <si>
-    <t>a.1.4</t>
+    <t>Title 6</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>a.1.6</t>
+  </si>
+  <si>
+    <t>PopesIIII</t>
+  </si>
+  <si>
+    <t>Title 7</t>
+  </si>
+  <si>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>a.1.7</t>
   </si>
   <si>
     <t>PopesInn</t>
   </si>
   <si>
-    <t>Title 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>a.1.5</t>
-  </si>
-  <si>
-    <t>PopesIIn</t>
-  </si>
-  <si>
-    <t>Title 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>a.1.6</t>
-  </si>
-  <si>
-    <t>PopesIII</t>
-  </si>
-  <si>
-    <t>Title 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>a.1.7</t>
-  </si>
-  <si>
-    <t>PopesIIIo</t>
-  </si>
-  <si>
     <t>Title 8</t>
   </si>
   <si>
@@ -158,7 +158,7 @@
     <t>a.1.8</t>
   </si>
   <si>
-    <t>PopesIIIon</t>
+    <t>PopesIIo</t>
   </si>
   <si>
     <t>Title 9</t>
@@ -170,181 +170,181 @@
     <t>a.1.9</t>
   </si>
   <si>
+    <t>PopesInnI</t>
+  </si>
+  <si>
+    <t>Title 10</t>
+  </si>
+  <si>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>a.1.0</t>
+  </si>
+  <si>
     <t>PopesIo</t>
   </si>
   <si>
-    <t>Title 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
-  </si>
-  <si>
-    <t>a.1.0</t>
+    <t>Title 11</t>
+  </si>
+  <si>
+    <t>Description 11</t>
+  </si>
+  <si>
+    <t>PopesIoo</t>
+  </si>
+  <si>
+    <t>Title 12</t>
+  </si>
+  <si>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>PopesIIoI</t>
+  </si>
+  <si>
+    <t>Title 13</t>
+  </si>
+  <si>
+    <t>Description 13</t>
+  </si>
+  <si>
+    <t>PopesIoon</t>
+  </si>
+  <si>
+    <t>Title 14</t>
+  </si>
+  <si>
+    <t>Description 14</t>
+  </si>
+  <si>
+    <t>PopesInnIn</t>
+  </si>
+  <si>
+    <t>Title 15</t>
+  </si>
+  <si>
+    <t>Description 15</t>
+  </si>
+  <si>
+    <t>PopesIno</t>
+  </si>
+  <si>
+    <t>Title 16</t>
+  </si>
+  <si>
+    <t>Description 16</t>
+  </si>
+  <si>
+    <t>PopesInno</t>
+  </si>
+  <si>
+    <t>Title 17</t>
+  </si>
+  <si>
+    <t>Description 17</t>
+  </si>
+  <si>
+    <t>PopesIoI</t>
+  </si>
+  <si>
+    <t>Title 18</t>
+  </si>
+  <si>
+    <t>Description 18</t>
+  </si>
+  <si>
+    <t>PopesIooo</t>
+  </si>
+  <si>
+    <t>Title 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>PopesIooI</t>
+  </si>
+  <si>
+    <t>Title 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
+  </si>
+  <si>
+    <t>PopesInnIo</t>
+  </si>
+  <si>
+    <t>Title 21</t>
+  </si>
+  <si>
+    <t>Description 21</t>
   </si>
   <si>
     <t>PopesIon</t>
   </si>
   <si>
-    <t>Title 11</t>
-  </si>
-  <si>
-    <t>Description 11</t>
-  </si>
-  <si>
-    <t>PopesInI</t>
-  </si>
-  <si>
-    <t>Title 12</t>
-  </si>
-  <si>
-    <t>Description 12</t>
-  </si>
-  <si>
-    <t>PopesIoI</t>
-  </si>
-  <si>
-    <t>Title 13</t>
-  </si>
-  <si>
-    <t>Description 13</t>
-  </si>
-  <si>
-    <t>PopesIoIo</t>
-  </si>
-  <si>
-    <t>Title 14</t>
-  </si>
-  <si>
-    <t>Description 14</t>
-  </si>
-  <si>
-    <t>PopesIno</t>
-  </si>
-  <si>
-    <t>Title 15</t>
-  </si>
-  <si>
-    <t>Description 15</t>
+    <t>Title 22</t>
+  </si>
+  <si>
+    <t>Description 22</t>
+  </si>
+  <si>
+    <t>PopesIIno</t>
+  </si>
+  <si>
+    <t>Title 23</t>
+  </si>
+  <si>
+    <t>Description 23</t>
   </si>
   <si>
     <t>PopesIoII</t>
   </si>
   <si>
-    <t>Title 16</t>
-  </si>
-  <si>
-    <t>Description 16</t>
-  </si>
-  <si>
-    <t>PopesInII</t>
-  </si>
-  <si>
-    <t>Title 17</t>
-  </si>
-  <si>
-    <t>Description 17</t>
-  </si>
-  <si>
-    <t>PopesIoIn</t>
-  </si>
-  <si>
-    <t>Title 18</t>
-  </si>
-  <si>
-    <t>Description 18</t>
+    <t>Title 24</t>
+  </si>
+  <si>
+    <t>Description 24</t>
   </si>
   <si>
     <t>PopesInnn</t>
   </si>
   <si>
-    <t>Title 19</t>
-  </si>
-  <si>
-    <t>Description 19</t>
-  </si>
-  <si>
-    <t>PopesIInn</t>
-  </si>
-  <si>
-    <t>Title 20</t>
-  </si>
-  <si>
-    <t>Description 20</t>
-  </si>
-  <si>
-    <t>PopesIIIn</t>
-  </si>
-  <si>
-    <t>Title 21</t>
-  </si>
-  <si>
-    <t>Description 21</t>
+    <t>Title 25</t>
+  </si>
+  <si>
+    <t>Description 25</t>
+  </si>
+  <si>
+    <t>PopesIIIIn</t>
+  </si>
+  <si>
+    <t>Title 26</t>
+  </si>
+  <si>
+    <t>Description 26</t>
+  </si>
+  <si>
+    <t>PopesIonn</t>
+  </si>
+  <si>
+    <t>Title 27</t>
+  </si>
+  <si>
+    <t>Description 27</t>
   </si>
   <si>
     <t>PopesIono</t>
   </si>
   <si>
-    <t>Title 22</t>
-  </si>
-  <si>
-    <t>Description 22</t>
-  </si>
-  <si>
-    <t>PopesInoI</t>
-  </si>
-  <si>
-    <t>Title 23</t>
-  </si>
-  <si>
-    <t>Description 23</t>
-  </si>
-  <si>
-    <t>PopesIoIoI</t>
-  </si>
-  <si>
-    <t>Title 24</t>
-  </si>
-  <si>
-    <t>Description 24</t>
-  </si>
-  <si>
-    <t>PopesInIIn</t>
-  </si>
-  <si>
-    <t>Title 25</t>
-  </si>
-  <si>
-    <t>Description 25</t>
-  </si>
-  <si>
-    <t>PopesInIn</t>
-  </si>
-  <si>
-    <t>Title 26</t>
-  </si>
-  <si>
-    <t>Description 26</t>
-  </si>
-  <si>
-    <t>PopesIIII</t>
-  </si>
-  <si>
-    <t>Title 27</t>
-  </si>
-  <si>
-    <t>Description 27</t>
-  </si>
-  <si>
-    <t>PopesIoo</t>
-  </si>
-  <si>
     <t>Title 28</t>
   </si>
   <si>
     <t>Description 28</t>
   </si>
   <si>
-    <t>PopesInno</t>
+    <t>PopesIIIII</t>
   </si>
   <si>
     <t>Title 29</t>
@@ -353,7 +353,7 @@
     <t>Description 29</t>
   </si>
   <si>
-    <t>PopesInnI</t>
+    <t>PopesIIon</t>
   </si>
   <si>
     <t>Title 30</t>
@@ -362,7 +362,7 @@
     <t>Description 30</t>
   </si>
   <si>
-    <t>PopesIooI</t>
+    <t>PopesIIonI</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" t="n" s="2">
-        <v>43321.656944375</v>
+        <v>43321.72465548611</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -495,13 +495,13 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -509,24 +509,24 @@
         <v>14.0</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="n" s="2">
-        <v>43321.656944675924</v>
+        <v>43321.72465585648</v>
       </c>
       <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
       <c r="I3" t="s">
         <v>23</v>
       </c>
@@ -534,7 +534,7 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -552,10 +552,10 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n" s="2">
-        <v>43321.65694497685</v>
+        <v>43321.72465621528</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
@@ -564,10 +564,10 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -585,7 +585,7 @@
       </c>
       <c r="E5"/>
       <c r="F5" t="n" s="2">
-        <v>43321.656945104165</v>
+        <v>43321.72465621528</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -594,13 +594,13 @@
         <v>32</v>
       </c>
       <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -618,22 +618,22 @@
       </c>
       <c r="E6"/>
       <c r="F6" t="n" s="2">
-        <v>43321.65694527778</v>
+        <v>43321.72465657407</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -651,7 +651,7 @@
       </c>
       <c r="E7"/>
       <c r="F7" t="n" s="2">
-        <v>43321.65694547454</v>
+        <v>43321.72465675926</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -660,13 +660,13 @@
         <v>40</v>
       </c>
       <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -684,22 +684,22 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n" s="2">
-        <v>43321.65694565972</v>
+        <v>43321.72465693287</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
         <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -717,22 +717,22 @@
       </c>
       <c r="E9"/>
       <c r="F9" t="n" s="2">
-        <v>43321.65694586805</v>
+        <v>43321.72465711806</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
         <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -750,22 +750,22 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n" s="2">
-        <v>43321.65694608796</v>
+        <v>43321.72465730324</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
         <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -783,22 +783,22 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n" s="2">
-        <v>43321.65694622685</v>
+        <v>43321.72465747685</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -816,22 +816,22 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n" s="2">
-        <v>43321.656946400464</v>
+        <v>43321.72465766204</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
         <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -845,26 +845,26 @@
         <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13"/>
       <c r="F13" t="n" s="2">
-        <v>43321.65694659722</v>
+        <v>43321.72465766204</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -882,10 +882,10 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n" s="2">
-        <v>43321.656946759256</v>
+        <v>43321.72465784722</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>65</v>
@@ -894,10 +894,10 @@
         <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -915,10 +915,10 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="n" s="2">
-        <v>43321.656946967596</v>
+        <v>43321.72465802083</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
         <v>68</v>
@@ -927,10 +927,10 @@
         <v>68</v>
       </c>
       <c r="J15" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -948,22 +948,22 @@
       </c>
       <c r="E16"/>
       <c r="F16" t="n" s="2">
-        <v>43321.65694712963</v>
+        <v>43321.72465820602</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H16" t="s">
         <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -981,22 +981,22 @@
       </c>
       <c r="E17"/>
       <c r="F17" t="n" s="2">
-        <v>43321.65694729167</v>
+        <v>43321.72465837963</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
         <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1014,10 +1014,10 @@
       </c>
       <c r="E18"/>
       <c r="F18" t="n" s="2">
-        <v>43321.65694746528</v>
+        <v>43321.72465856482</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
         <v>77</v>
@@ -1026,10 +1026,10 @@
         <v>77</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1047,10 +1047,10 @@
       </c>
       <c r="E19"/>
       <c r="F19" t="n" s="2">
-        <v>43321.656947627314</v>
+        <v>43321.72465875</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
@@ -1059,10 +1059,10 @@
         <v>80</v>
       </c>
       <c r="J19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -1080,22 +1080,22 @@
       </c>
       <c r="E20"/>
       <c r="F20" t="n" s="2">
-        <v>43321.65694777778</v>
+        <v>43321.72465875</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" t="s">
         <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="J20" t="s">
         <v>24</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -1113,22 +1113,22 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n" s="2">
-        <v>43321.65694793982</v>
+        <v>43321.72465892361</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H21" t="s">
         <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="E22"/>
       <c r="F22" t="n" s="2">
-        <v>43321.65694811343</v>
+        <v>43321.724659293985</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1155,13 +1155,13 @@
         <v>89</v>
       </c>
       <c r="I22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" t="s">
         <v>16</v>
       </c>
-      <c r="J22" t="s">
-        <v>17</v>
-      </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
@@ -1175,26 +1175,26 @@
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23"/>
       <c r="F23" t="n" s="2">
-        <v>43321.65694825231</v>
+        <v>43321.724659293985</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" t="s">
         <v>92</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="J23" t="s">
         <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
@@ -1212,22 +1212,22 @@
       </c>
       <c r="E24"/>
       <c r="F24" t="n" s="2">
-        <v>43321.65694849537</v>
+        <v>43321.724659467596</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H24" t="s">
         <v>95</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -1245,22 +1245,22 @@
       </c>
       <c r="E25"/>
       <c r="F25" t="n" s="2">
-        <v>43321.656948703705</v>
+        <v>43321.72465965278</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H25" t="s">
         <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="E26"/>
       <c r="F26" t="n" s="2">
-        <v>43321.656948888885</v>
+        <v>43321.72465982639</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
@@ -1287,13 +1287,13 @@
         <v>101</v>
       </c>
       <c r="I26" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26" t="s">
         <v>16</v>
       </c>
-      <c r="J26" t="s">
-        <v>17</v>
-      </c>
       <c r="K26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
@@ -1311,10 +1311,10 @@
       </c>
       <c r="E27"/>
       <c r="F27" t="n" s="2">
-        <v>43321.65694903935</v>
+        <v>43321.724660011576</v>
       </c>
       <c r="G27" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s">
         <v>104</v>
@@ -1323,10 +1323,10 @@
         <v>104</v>
       </c>
       <c r="J27" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
@@ -1344,10 +1344,10 @@
       </c>
       <c r="E28"/>
       <c r="F28" t="n" s="2">
-        <v>43321.65694920139</v>
+        <v>43321.724660196756</v>
       </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
         <v>107</v>
@@ -1356,10 +1356,10 @@
         <v>107</v>
       </c>
       <c r="J28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
@@ -1377,22 +1377,22 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n" s="2">
-        <v>43321.6569493287</v>
+        <v>43321.72466037037</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H29" t="s">
         <v>110</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
@@ -1410,22 +1410,22 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n" s="2">
-        <v>43321.65694949074</v>
+        <v>43321.724660555556</v>
       </c>
       <c r="G30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H30" t="s">
         <v>113</v>
       </c>
       <c r="I30" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="J30" t="s">
         <v>24</v>
       </c>
       <c r="K30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1443,22 +1443,22 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n" s="2">
-        <v>43321.656949641205</v>
+        <v>43321.72466074074</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H31" t="s">
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pdf is looking better
</commit_message>
<xml_diff>
--- a/ExcelBugs.xlsx
+++ b/ExcelBugs.xlsx
@@ -83,277 +83,277 @@
     <t>CRITICAL</t>
   </si>
   <si>
+    <t>PopesIn</t>
+  </si>
+  <si>
+    <t>IN_PROGRESS</t>
+  </si>
+  <si>
+    <t>Title 3</t>
+  </si>
+  <si>
+    <t>Description 3</t>
+  </si>
+  <si>
+    <t>a.1.3</t>
+  </si>
+  <si>
+    <t>PopesInI</t>
+  </si>
+  <si>
+    <t>Title 4</t>
+  </si>
+  <si>
+    <t>Description 4</t>
+  </si>
+  <si>
+    <t>a.1.4</t>
+  </si>
+  <si>
+    <t>PopesIo</t>
+  </si>
+  <si>
+    <t>Title 5</t>
+  </si>
+  <si>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>a.1.5</t>
+  </si>
+  <si>
     <t>PopesII</t>
   </si>
   <si>
-    <t>IN_PROGRESS</t>
-  </si>
-  <si>
-    <t>Title 3</t>
-  </si>
-  <si>
-    <t>Description 3</t>
-  </si>
-  <si>
-    <t>a.1.3</t>
-  </si>
-  <si>
-    <t>PopesIo</t>
-  </si>
-  <si>
-    <t>Title 4</t>
-  </si>
-  <si>
-    <t>Description 4</t>
-  </si>
-  <si>
-    <t>a.1.4</t>
+    <t>Title 6</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>a.1.6</t>
+  </si>
+  <si>
+    <t>PopesIoI</t>
+  </si>
+  <si>
+    <t>Title 7</t>
+  </si>
+  <si>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>a.1.7</t>
+  </si>
+  <si>
+    <t>PopesIoo</t>
+  </si>
+  <si>
+    <t>Title 8</t>
+  </si>
+  <si>
+    <t>Description 8</t>
+  </si>
+  <si>
+    <t>a.1.8</t>
   </si>
   <si>
     <t>PopesIIn</t>
   </si>
   <si>
-    <t>Title 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>a.1.5</t>
-  </si>
-  <si>
-    <t>PopesIn</t>
-  </si>
-  <si>
-    <t>Title 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>a.1.6</t>
+    <t>Title 9</t>
+  </si>
+  <si>
+    <t>Description 9</t>
+  </si>
+  <si>
+    <t>a.1.9</t>
+  </si>
+  <si>
+    <t>PopesIooI</t>
+  </si>
+  <si>
+    <t>Title 10</t>
+  </si>
+  <si>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>a.1.0</t>
   </si>
   <si>
     <t>PopesIno</t>
   </si>
   <si>
-    <t>Title 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>a.1.7</t>
-  </si>
-  <si>
-    <t>PopesIoo</t>
-  </si>
-  <si>
-    <t>Title 8</t>
-  </si>
-  <si>
-    <t>Description 8</t>
-  </si>
-  <si>
-    <t>a.1.8</t>
+    <t>Title 11</t>
+  </si>
+  <si>
+    <t>Description 11</t>
+  </si>
+  <si>
+    <t>PopesIInn</t>
+  </si>
+  <si>
+    <t>Title 12</t>
+  </si>
+  <si>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>PopesInoo</t>
+  </si>
+  <si>
+    <t>Title 13</t>
+  </si>
+  <si>
+    <t>Description 13</t>
+  </si>
+  <si>
+    <t>PopesIooo</t>
+  </si>
+  <si>
+    <t>Title 14</t>
+  </si>
+  <si>
+    <t>Description 14</t>
+  </si>
+  <si>
+    <t>PopesInIo</t>
+  </si>
+  <si>
+    <t>Title 15</t>
+  </si>
+  <si>
+    <t>Description 15</t>
+  </si>
+  <si>
+    <t>PopesIoon</t>
+  </si>
+  <si>
+    <t>Title 16</t>
+  </si>
+  <si>
+    <t>Description 16</t>
+  </si>
+  <si>
+    <t>PopesIoIn</t>
+  </si>
+  <si>
+    <t>Title 17</t>
+  </si>
+  <si>
+    <t>Description 17</t>
+  </si>
+  <si>
+    <t>PopesInn</t>
+  </si>
+  <si>
+    <t>Title 18</t>
+  </si>
+  <si>
+    <t>Description 18</t>
+  </si>
+  <si>
+    <t>PopesIoooo</t>
+  </si>
+  <si>
+    <t>Title 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>PopesIoII</t>
+  </si>
+  <si>
+    <t>Title 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
+  </si>
+  <si>
+    <t>PopesIooon</t>
+  </si>
+  <si>
+    <t>Title 21</t>
+  </si>
+  <si>
+    <t>Description 21</t>
   </si>
   <si>
     <t>PopesIIno</t>
   </si>
   <si>
-    <t>Title 9</t>
-  </si>
-  <si>
-    <t>Description 9</t>
-  </si>
-  <si>
-    <t>a.1.9</t>
-  </si>
-  <si>
-    <t>PopesInn</t>
-  </si>
-  <si>
-    <t>Title 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
-  </si>
-  <si>
-    <t>a.1.0</t>
-  </si>
-  <si>
-    <t>PopesIooo</t>
-  </si>
-  <si>
-    <t>Title 11</t>
-  </si>
-  <si>
-    <t>Description 11</t>
+    <t>Title 22</t>
+  </si>
+  <si>
+    <t>Description 22</t>
+  </si>
+  <si>
+    <t>PopesInoI</t>
+  </si>
+  <si>
+    <t>Title 23</t>
+  </si>
+  <si>
+    <t>Description 23</t>
+  </si>
+  <si>
+    <t>PopesIInnI</t>
+  </si>
+  <si>
+    <t>Title 24</t>
+  </si>
+  <si>
+    <t>Description 24</t>
+  </si>
+  <si>
+    <t>PopesIIo</t>
+  </si>
+  <si>
+    <t>Title 25</t>
+  </si>
+  <si>
+    <t>Description 25</t>
+  </si>
+  <si>
+    <t>PopesIInoI</t>
+  </si>
+  <si>
+    <t>Title 26</t>
+  </si>
+  <si>
+    <t>Description 26</t>
+  </si>
+  <si>
+    <t>PopesInno</t>
+  </si>
+  <si>
+    <t>Title 27</t>
+  </si>
+  <si>
+    <t>Description 27</t>
   </si>
   <si>
     <t>PopesInon</t>
   </si>
   <si>
-    <t>Title 12</t>
-  </si>
-  <si>
-    <t>Description 12</t>
-  </si>
-  <si>
-    <t>PopesIII</t>
-  </si>
-  <si>
-    <t>Title 13</t>
-  </si>
-  <si>
-    <t>Description 13</t>
-  </si>
-  <si>
-    <t>PopesIIIo</t>
-  </si>
-  <si>
-    <t>Title 14</t>
-  </si>
-  <si>
-    <t>Description 14</t>
+    <t>Title 28</t>
+  </si>
+  <si>
+    <t>Description 28</t>
   </si>
   <si>
     <t>PopesIon</t>
   </si>
   <si>
-    <t>Title 15</t>
-  </si>
-  <si>
-    <t>Description 15</t>
-  </si>
-  <si>
-    <t>PopesIooI</t>
-  </si>
-  <si>
-    <t>Title 16</t>
-  </si>
-  <si>
-    <t>Description 16</t>
-  </si>
-  <si>
-    <t>PopesIIo</t>
-  </si>
-  <si>
-    <t>Title 17</t>
-  </si>
-  <si>
-    <t>Description 17</t>
-  </si>
-  <si>
-    <t>PopesIIon</t>
-  </si>
-  <si>
-    <t>Title 18</t>
-  </si>
-  <si>
-    <t>Description 18</t>
-  </si>
-  <si>
-    <t>PopesInI</t>
-  </si>
-  <si>
-    <t>Title 19</t>
-  </si>
-  <si>
-    <t>Description 19</t>
-  </si>
-  <si>
-    <t>PopesIIoo</t>
-  </si>
-  <si>
-    <t>Title 20</t>
-  </si>
-  <si>
-    <t>Description 20</t>
-  </si>
-  <si>
-    <t>PopesInII</t>
-  </si>
-  <si>
-    <t>Title 21</t>
-  </si>
-  <si>
-    <t>Description 21</t>
-  </si>
-  <si>
-    <t>PopesIIIon</t>
-  </si>
-  <si>
-    <t>Title 22</t>
-  </si>
-  <si>
-    <t>Description 22</t>
-  </si>
-  <si>
-    <t>PopesInIo</t>
-  </si>
-  <si>
-    <t>Title 23</t>
-  </si>
-  <si>
-    <t>Description 23</t>
-  </si>
-  <si>
-    <t>PopesInonn</t>
-  </si>
-  <si>
-    <t>Title 24</t>
-  </si>
-  <si>
-    <t>Description 24</t>
-  </si>
-  <si>
-    <t>PopesInoI</t>
-  </si>
-  <si>
-    <t>Title 25</t>
-  </si>
-  <si>
-    <t>Description 25</t>
-  </si>
-  <si>
-    <t>PopesIoooo</t>
-  </si>
-  <si>
-    <t>Title 26</t>
-  </si>
-  <si>
-    <t>Description 26</t>
-  </si>
-  <si>
-    <t>PopesIInn</t>
-  </si>
-  <si>
-    <t>Title 27</t>
-  </si>
-  <si>
-    <t>Description 27</t>
-  </si>
-  <si>
-    <t>PopesInIn</t>
-  </si>
-  <si>
-    <t>Title 28</t>
-  </si>
-  <si>
-    <t>Description 28</t>
-  </si>
-  <si>
-    <t>PopesIInno</t>
-  </si>
-  <si>
     <t>Title 29</t>
   </si>
   <si>
     <t>Description 29</t>
   </si>
   <si>
-    <t>PopesIoI</t>
+    <t>PopesIonI</t>
   </si>
   <si>
     <t>Title 30</t>
@@ -362,7 +362,7 @@
     <t>Description 30</t>
   </si>
   <si>
-    <t>PopesIooIo</t>
+    <t>PopesIInI</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" t="n" s="2">
-        <v>43321.73177396991</v>
+        <v>43322.56793877315</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -519,7 +519,7 @@
       </c>
       <c r="E3"/>
       <c r="F3" t="n" s="2">
-        <v>43321.731774155094</v>
+        <v>43322.56793895833</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -552,7 +552,7 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n" s="2">
-        <v>43321.731774513886</v>
+        <v>43322.56793931713</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -585,7 +585,7 @@
       </c>
       <c r="E5"/>
       <c r="F5" t="n" s="2">
-        <v>43321.731774699074</v>
+        <v>43322.56793950232</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -618,7 +618,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" t="n" s="2">
-        <v>43321.73177488426</v>
+        <v>43322.56793950232</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -651,19 +651,19 @@
       </c>
       <c r="E7"/>
       <c r="F7" t="n" s="2">
-        <v>43321.73177505787</v>
+        <v>43322.56793967592</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
@@ -684,19 +684,19 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n" s="2">
-        <v>43321.73177524305</v>
+        <v>43322.56794003472</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
         <v>18</v>
@@ -717,19 +717,19 @@
       </c>
       <c r="E9"/>
       <c r="F9" t="n" s="2">
-        <v>43321.73177560185</v>
+        <v>43322.56794021991</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K9" t="s">
         <v>18</v>
@@ -750,7 +750,7 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n" s="2">
-        <v>43321.73177578704</v>
+        <v>43322.56794040509</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -783,19 +783,19 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n" s="2">
-        <v>43321.731775960645</v>
+        <v>43322.5679405787</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K11" t="s">
         <v>18</v>
@@ -816,19 +816,19 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n" s="2">
-        <v>43321.73177633102</v>
+        <v>43322.56794076389</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
         <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
@@ -849,19 +849,19 @@
       </c>
       <c r="E13"/>
       <c r="F13" t="n" s="2">
-        <v>43321.73177633102</v>
+        <v>43322.56794112269</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
@@ -882,7 +882,7 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n" s="2">
-        <v>43321.73177650463</v>
+        <v>43322.56794130787</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="n" s="2">
-        <v>43321.731776863424</v>
+        <v>43322.56794148148</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -948,19 +948,19 @@
       </c>
       <c r="E16"/>
       <c r="F16" t="n" s="2">
-        <v>43321.73177704861</v>
+        <v>43322.56794166667</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
         <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K16" t="s">
         <v>18</v>
@@ -981,7 +981,7 @@
       </c>
       <c r="E17"/>
       <c r="F17" t="n" s="2">
-        <v>43321.7317772338</v>
+        <v>43322.56794185185</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
@@ -1014,19 +1014,19 @@
       </c>
       <c r="E18"/>
       <c r="F18" t="n" s="2">
-        <v>43321.73177740741</v>
+        <v>43322.56794202546</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
         <v>77</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
         <v>18</v>
@@ -1047,19 +1047,19 @@
       </c>
       <c r="E19"/>
       <c r="F19" t="n" s="2">
-        <v>43321.73177759259</v>
+        <v>43322.56794202546</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -1080,19 +1080,19 @@
       </c>
       <c r="E20"/>
       <c r="F20" t="n" s="2">
-        <v>43321.73177777778</v>
+        <v>43322.56794221065</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H20" t="s">
         <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
@@ -1113,19 +1113,19 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n" s="2">
-        <v>43321.73177795139</v>
+        <v>43322.56794256945</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
         <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="E22"/>
       <c r="F22" t="n" s="2">
-        <v>43321.73177813657</v>
+        <v>43322.56794275463</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E23"/>
       <c r="F23" t="n" s="2">
-        <v>43321.73177831018</v>
+        <v>43322.56794292824</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -1212,19 +1212,19 @@
       </c>
       <c r="E24"/>
       <c r="F24" t="n" s="2">
-        <v>43321.73177849537</v>
+        <v>43322.56794311343</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
         <v>95</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K24" t="s">
         <v>18</v>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E25"/>
       <c r="F25" t="n" s="2">
-        <v>43321.73177868056</v>
+        <v>43322.567943298614</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -1278,19 +1278,19 @@
       </c>
       <c r="E26"/>
       <c r="F26" t="n" s="2">
-        <v>43321.73177885417</v>
+        <v>43322.56794347222</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H26" t="s">
         <v>101</v>
       </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -1311,19 +1311,19 @@
       </c>
       <c r="E27"/>
       <c r="F27" t="n" s="2">
-        <v>43321.73177922454</v>
+        <v>43322.56794365741</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H27" t="s">
         <v>104</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K27" t="s">
         <v>18</v>
@@ -1344,19 +1344,19 @@
       </c>
       <c r="E28"/>
       <c r="F28" t="n" s="2">
-        <v>43321.73177939815</v>
+        <v>43322.567943842594</v>
       </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
         <v>107</v>
       </c>
       <c r="I28" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="J28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K28" t="s">
         <v>18</v>
@@ -1377,19 +1377,19 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n" s="2">
-        <v>43321.73177958334</v>
+        <v>43322.567944016206</v>
       </c>
       <c r="G29" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
         <v>110</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -1410,19 +1410,19 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n" s="2">
-        <v>43321.73177976852</v>
+        <v>43322.567944201386</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H30" t="s">
         <v>113</v>
       </c>
       <c r="I30" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="J30" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K30" t="s">
         <v>18</v>
@@ -1443,19 +1443,19 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n" s="2">
-        <v>43321.73177994213</v>
+        <v>43322.567944375</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H31" t="s">
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
notification table to homepage
</commit_message>
<xml_diff>
--- a/ExcelBugs.xlsx
+++ b/ExcelBugs.xlsx
@@ -98,127 +98,127 @@
     <t>a.1.3</t>
   </si>
   <si>
+    <t>PopesIn</t>
+  </si>
+  <si>
+    <t>Title 4</t>
+  </si>
+  <si>
+    <t>Description 4</t>
+  </si>
+  <si>
+    <t>a.1.4</t>
+  </si>
+  <si>
+    <t>PopesIII</t>
+  </si>
+  <si>
+    <t>Title 5</t>
+  </si>
+  <si>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>a.1.5</t>
+  </si>
+  <si>
+    <t>PopesIIo</t>
+  </si>
+  <si>
+    <t>Title 6</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>a.1.6</t>
+  </si>
+  <si>
+    <t>PopesIIIn</t>
+  </si>
+  <si>
+    <t>Title 7</t>
+  </si>
+  <si>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>a.1.7</t>
+  </si>
+  <si>
+    <t>PopesIno</t>
+  </si>
+  <si>
+    <t>Title 8</t>
+  </si>
+  <si>
+    <t>Description 8</t>
+  </si>
+  <si>
+    <t>a.1.8</t>
+  </si>
+  <si>
+    <t>PopesInn</t>
+  </si>
+  <si>
+    <t>Title 9</t>
+  </si>
+  <si>
+    <t>Description 9</t>
+  </si>
+  <si>
+    <t>a.1.9</t>
+  </si>
+  <si>
     <t>PopesIo</t>
   </si>
   <si>
-    <t>Title 4</t>
-  </si>
-  <si>
-    <t>Description 4</t>
-  </si>
-  <si>
-    <t>a.1.4</t>
+    <t>Title 10</t>
+  </si>
+  <si>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>a.1.0</t>
+  </si>
+  <si>
+    <t>PopesIon</t>
+  </si>
+  <si>
+    <t>Title 11</t>
+  </si>
+  <si>
+    <t>Description 11</t>
   </si>
   <si>
     <t>PopesIIn</t>
   </si>
   <si>
-    <t>Title 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>a.1.5</t>
-  </si>
-  <si>
-    <t>PopesIn</t>
-  </si>
-  <si>
-    <t>Title 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>a.1.6</t>
-  </si>
-  <si>
-    <t>PopesIno</t>
-  </si>
-  <si>
-    <t>Title 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>a.1.7</t>
+    <t>Title 12</t>
+  </si>
+  <si>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>PopesIIoo</t>
+  </si>
+  <si>
+    <t>Title 13</t>
+  </si>
+  <si>
+    <t>Description 13</t>
   </si>
   <si>
     <t>PopesIoo</t>
   </si>
   <si>
-    <t>Title 8</t>
-  </si>
-  <si>
-    <t>Description 8</t>
-  </si>
-  <si>
-    <t>a.1.8</t>
-  </si>
-  <si>
-    <t>PopesIIno</t>
-  </si>
-  <si>
-    <t>Title 9</t>
-  </si>
-  <si>
-    <t>Description 9</t>
-  </si>
-  <si>
-    <t>a.1.9</t>
-  </si>
-  <si>
-    <t>PopesInn</t>
-  </si>
-  <si>
-    <t>Title 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
-  </si>
-  <si>
-    <t>a.1.0</t>
-  </si>
-  <si>
-    <t>PopesIooo</t>
-  </si>
-  <si>
-    <t>Title 11</t>
-  </si>
-  <si>
-    <t>Description 11</t>
-  </si>
-  <si>
-    <t>PopesInon</t>
-  </si>
-  <si>
-    <t>Title 12</t>
-  </si>
-  <si>
-    <t>Description 12</t>
-  </si>
-  <si>
-    <t>PopesIII</t>
-  </si>
-  <si>
-    <t>Title 13</t>
-  </si>
-  <si>
-    <t>Description 13</t>
-  </si>
-  <si>
-    <t>PopesIIIo</t>
-  </si>
-  <si>
     <t>Title 14</t>
   </si>
   <si>
     <t>Description 14</t>
   </si>
   <si>
-    <t>PopesIon</t>
+    <t>PopesIInn</t>
   </si>
   <si>
     <t>Title 15</t>
@@ -227,7 +227,7 @@
     <t>Description 15</t>
   </si>
   <si>
-    <t>PopesIooI</t>
+    <t>PopesInoo</t>
   </si>
   <si>
     <t>Title 16</t>
@@ -236,7 +236,7 @@
     <t>Description 16</t>
   </si>
   <si>
-    <t>PopesIIo</t>
+    <t>PopesIIon</t>
   </si>
   <si>
     <t>Title 17</t>
@@ -245,7 +245,7 @@
     <t>Description 17</t>
   </si>
   <si>
-    <t>PopesIIon</t>
+    <t>PopesIIIno</t>
   </si>
   <si>
     <t>Title 18</t>
@@ -254,43 +254,43 @@
     <t>Description 18</t>
   </si>
   <si>
+    <t>PopesIono</t>
+  </si>
+  <si>
+    <t>Title 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>PopesIInnI</t>
+  </si>
+  <si>
+    <t>Title 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
+  </si>
+  <si>
+    <t>PopesInno</t>
+  </si>
+  <si>
+    <t>Title 21</t>
+  </si>
+  <si>
+    <t>Description 21</t>
+  </si>
+  <si>
     <t>PopesInI</t>
   </si>
   <si>
-    <t>Title 19</t>
-  </si>
-  <si>
-    <t>Description 19</t>
-  </si>
-  <si>
-    <t>PopesIIoo</t>
-  </si>
-  <si>
-    <t>Title 20</t>
-  </si>
-  <si>
-    <t>Description 20</t>
-  </si>
-  <si>
-    <t>PopesInII</t>
-  </si>
-  <si>
-    <t>Title 21</t>
-  </si>
-  <si>
-    <t>Description 21</t>
-  </si>
-  <si>
-    <t>PopesIIIon</t>
-  </si>
-  <si>
     <t>Title 22</t>
   </si>
   <si>
     <t>Description 22</t>
   </si>
   <si>
-    <t>PopesInIo</t>
+    <t>PopesIIooo</t>
   </si>
   <si>
     <t>Title 23</t>
@@ -299,7 +299,7 @@
     <t>Description 23</t>
   </si>
   <si>
-    <t>PopesInonn</t>
+    <t>PopesInoI</t>
   </si>
   <si>
     <t>Title 24</t>
@@ -308,7 +308,7 @@
     <t>Description 24</t>
   </si>
   <si>
-    <t>PopesInoI</t>
+    <t>PopesIIoon</t>
   </si>
   <si>
     <t>Title 25</t>
@@ -317,7 +317,7 @@
     <t>Description 25</t>
   </si>
   <si>
-    <t>PopesIoooo</t>
+    <t>PopesIoon</t>
   </si>
   <si>
     <t>Title 26</t>
@@ -326,7 +326,7 @@
     <t>Description 26</t>
   </si>
   <si>
-    <t>PopesIInn</t>
+    <t>PopesIInnII</t>
   </si>
   <si>
     <t>Title 27</t>
@@ -335,7 +335,7 @@
     <t>Description 27</t>
   </si>
   <si>
-    <t>PopesInIn</t>
+    <t>PopesInnoI</t>
   </si>
   <si>
     <t>Title 28</t>
@@ -344,7 +344,7 @@
     <t>Description 28</t>
   </si>
   <si>
-    <t>PopesIInno</t>
+    <t>PopesIoI</t>
   </si>
   <si>
     <t>Title 29</t>
@@ -353,7 +353,7 @@
     <t>Description 29</t>
   </si>
   <si>
-    <t>PopesIoI</t>
+    <t>PopesInnI</t>
   </si>
   <si>
     <t>Title 30</t>
@@ -362,7 +362,7 @@
     <t>Description 30</t>
   </si>
   <si>
-    <t>PopesIooIo</t>
+    <t>PopesIInI</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" t="n" s="2">
-        <v>43321.73177396991</v>
+        <v>43322.58619372685</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -519,7 +519,7 @@
       </c>
       <c r="E3"/>
       <c r="F3" t="n" s="2">
-        <v>43321.731774155094</v>
+        <v>43322.58619408565</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>22.0</v>
+        <v>25.0</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -552,19 +552,19 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n" s="2">
-        <v>43321.731774513886</v>
+        <v>43322.58619425926</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>30.0</v>
+        <v>34.0</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
@@ -585,7 +585,7 @@
       </c>
       <c r="E5"/>
       <c r="F5" t="n" s="2">
-        <v>43321.731774699074</v>
+        <v>43322.58619444445</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>38.0</v>
+        <v>43.0</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -618,7 +618,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" t="n" s="2">
-        <v>43321.73177488426</v>
+        <v>43322.58619462963</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -651,7 +651,7 @@
       </c>
       <c r="E7"/>
       <c r="F7" t="n" s="2">
-        <v>43321.73177505787</v>
+        <v>43322.58619480324</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>54.0</v>
+        <v>61.0</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
@@ -684,7 +684,7 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n" s="2">
-        <v>43321.73177524305</v>
+        <v>43322.58619498843</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>62.0</v>
+        <v>70.0</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
@@ -717,7 +717,7 @@
       </c>
       <c r="E9"/>
       <c r="F9" t="n" s="2">
-        <v>43321.73177560185</v>
+        <v>43322.58619517361</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>70.0</v>
+        <v>79.0</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -750,7 +750,7 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n" s="2">
-        <v>43321.73177578704</v>
+        <v>43322.58619534722</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>78.0</v>
+        <v>88.0</v>
       </c>
       <c r="B11" t="s">
         <v>53</v>
@@ -783,19 +783,19 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n" s="2">
-        <v>43321.731775960645</v>
+        <v>43322.58619553241</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K11" t="s">
         <v>18</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>86.0</v>
+        <v>97.0</v>
       </c>
       <c r="B12" t="s">
         <v>57</v>
@@ -816,7 +816,7 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n" s="2">
-        <v>43321.73177633102</v>
+        <v>43322.58619570602</v>
       </c>
       <c r="G12" t="s">
         <v>22</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>94.0</v>
+        <v>106.0</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
@@ -849,7 +849,7 @@
       </c>
       <c r="E13"/>
       <c r="F13" t="n" s="2">
-        <v>43321.73177633102</v>
+        <v>43322.58619589121</v>
       </c>
       <c r="G13" t="s">
         <v>22</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>102.0</v>
+        <v>115.0</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
@@ -882,7 +882,7 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n" s="2">
-        <v>43321.73177650463</v>
+        <v>43322.58619607639</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>110.0</v>
+        <v>124.0</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
@@ -915,19 +915,19 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="n" s="2">
-        <v>43321.731776863424</v>
+        <v>43322.58619625</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
         <v>68</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
         <v>18</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>118.0</v>
+        <v>133.0</v>
       </c>
       <c r="B16" t="s">
         <v>69</v>
@@ -948,7 +948,7 @@
       </c>
       <c r="E16"/>
       <c r="F16" t="n" s="2">
-        <v>43321.73177704861</v>
+        <v>43322.586196435186</v>
       </c>
       <c r="G16" t="s">
         <v>22</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>126.0</v>
+        <v>142.0</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
@@ -981,19 +981,19 @@
       </c>
       <c r="E17"/>
       <c r="F17" t="n" s="2">
-        <v>43321.7317772338</v>
+        <v>43322.58619679398</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
         <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K17" t="s">
         <v>18</v>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>134.0</v>
+        <v>151.0</v>
       </c>
       <c r="B18" t="s">
         <v>75</v>
@@ -1014,19 +1014,19 @@
       </c>
       <c r="E18"/>
       <c r="F18" t="n" s="2">
-        <v>43321.73177740741</v>
+        <v>43322.586196979166</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
         <v>77</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
         <v>18</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>142.0</v>
+        <v>160.0</v>
       </c>
       <c r="B19" t="s">
         <v>78</v>
@@ -1047,19 +1047,19 @@
       </c>
       <c r="E19"/>
       <c r="F19" t="n" s="2">
-        <v>43321.73177759259</v>
+        <v>43322.58619715278</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>150.0</v>
+        <v>169.0</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E20"/>
       <c r="F20" t="n" s="2">
-        <v>43321.73177777778</v>
+        <v>43322.586197337965</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>158.0</v>
+        <v>178.0</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -1113,19 +1113,19 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n" s="2">
-        <v>43321.73177795139</v>
+        <v>43322.586197523146</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
         <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>166.0</v>
+        <v>187.0</v>
       </c>
       <c r="B22" t="s">
         <v>87</v>
@@ -1146,19 +1146,19 @@
       </c>
       <c r="E22"/>
       <c r="F22" t="n" s="2">
-        <v>43321.73177813657</v>
+        <v>43322.586197881945</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s">
         <v>89</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>174.0</v>
+        <v>196.0</v>
       </c>
       <c r="B23" t="s">
         <v>90</v>
@@ -1179,19 +1179,19 @@
       </c>
       <c r="E23"/>
       <c r="F23" t="n" s="2">
-        <v>43321.73177831018</v>
+        <v>43322.58619806713</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H23" t="s">
         <v>92</v>
       </c>
       <c r="I23" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>182.0</v>
+        <v>205.0</v>
       </c>
       <c r="B24" t="s">
         <v>93</v>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="E24"/>
       <c r="F24" t="n" s="2">
-        <v>43321.73177849537</v>
+        <v>43322.586198240744</v>
       </c>
       <c r="G24" t="s">
         <v>22</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>190.0</v>
+        <v>214.0</v>
       </c>
       <c r="B25" t="s">
         <v>96</v>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E25"/>
       <c r="F25" t="n" s="2">
-        <v>43321.73177868056</v>
+        <v>43322.586198425925</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>198.0</v>
+        <v>223.0</v>
       </c>
       <c r="B26" t="s">
         <v>99</v>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="E26"/>
       <c r="F26" t="n" s="2">
-        <v>43321.73177885417</v>
+        <v>43322.586198599536</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>206.0</v>
+        <v>232.0</v>
       </c>
       <c r="B27" t="s">
         <v>102</v>
@@ -1311,19 +1311,19 @@
       </c>
       <c r="E27"/>
       <c r="F27" t="n" s="2">
-        <v>43321.73177922454</v>
+        <v>43322.586198784724</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H27" t="s">
         <v>104</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K27" t="s">
         <v>18</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>214.0</v>
+        <v>241.0</v>
       </c>
       <c r="B28" t="s">
         <v>105</v>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E28"/>
       <c r="F28" t="n" s="2">
-        <v>43321.73177939815</v>
+        <v>43322.586198969904</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>222.0</v>
+        <v>250.0</v>
       </c>
       <c r="B29" t="s">
         <v>108</v>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n" s="2">
-        <v>43321.73177958334</v>
+        <v>43322.586199143516</v>
       </c>
       <c r="G29" t="s">
         <v>22</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>230.0</v>
+        <v>259.0</v>
       </c>
       <c r="B30" t="s">
         <v>111</v>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n" s="2">
-        <v>43321.73177976852</v>
+        <v>43322.5861993287</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>238.0</v>
+        <v>268.0</v>
       </c>
       <c r="B31" t="s">
         <v>114</v>
@@ -1443,19 +1443,19 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n" s="2">
-        <v>43321.73177994213</v>
+        <v>43322.58619951389</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H31" t="s">
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
tracks old and new info updated
</commit_message>
<xml_diff>
--- a/ExcelBugs.xlsx
+++ b/ExcelBugs.xlsx
@@ -83,268 +83,268 @@
     <t>CRITICAL</t>
   </si>
   <si>
+    <t>PopesIo</t>
+  </si>
+  <si>
+    <t>IN_PROGRESS</t>
+  </si>
+  <si>
+    <t>Title 3</t>
+  </si>
+  <si>
+    <t>Description 3</t>
+  </si>
+  <si>
+    <t>a.1.3</t>
+  </si>
+  <si>
+    <t>PopesIn</t>
+  </si>
+  <si>
+    <t>Title 4</t>
+  </si>
+  <si>
+    <t>Description 4</t>
+  </si>
+  <si>
+    <t>a.1.4</t>
+  </si>
+  <si>
+    <t>PopesIno</t>
+  </si>
+  <si>
+    <t>Title 5</t>
+  </si>
+  <si>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>a.1.5</t>
+  </si>
+  <si>
+    <t>PopesInoo</t>
+  </si>
+  <si>
+    <t>Title 6</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>a.1.6</t>
+  </si>
+  <si>
+    <t>PopesInI</t>
+  </si>
+  <si>
+    <t>Title 7</t>
+  </si>
+  <si>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>a.1.7</t>
+  </si>
+  <si>
+    <t>PopesIoo</t>
+  </si>
+  <si>
+    <t>Title 8</t>
+  </si>
+  <si>
+    <t>Description 8</t>
+  </si>
+  <si>
+    <t>a.1.8</t>
+  </si>
+  <si>
     <t>PopesII</t>
   </si>
   <si>
-    <t>IN_PROGRESS</t>
-  </si>
-  <si>
-    <t>Title 3</t>
-  </si>
-  <si>
-    <t>Description 3</t>
-  </si>
-  <si>
-    <t>a.1.3</t>
-  </si>
-  <si>
-    <t>PopesIn</t>
-  </si>
-  <si>
-    <t>Title 4</t>
-  </si>
-  <si>
-    <t>Description 4</t>
-  </si>
-  <si>
-    <t>a.1.4</t>
+    <t>Title 9</t>
+  </si>
+  <si>
+    <t>Description 9</t>
+  </si>
+  <si>
+    <t>a.1.9</t>
+  </si>
+  <si>
+    <t>PopesIoI</t>
+  </si>
+  <si>
+    <t>Title 10</t>
+  </si>
+  <si>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>a.1.0</t>
+  </si>
+  <si>
+    <t>PopesIoIo</t>
+  </si>
+  <si>
+    <t>Title 11</t>
+  </si>
+  <si>
+    <t>Description 11</t>
+  </si>
+  <si>
+    <t>PopesIIn</t>
+  </si>
+  <si>
+    <t>Title 12</t>
+  </si>
+  <si>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>PopesIoIoo</t>
+  </si>
+  <si>
+    <t>Title 13</t>
+  </si>
+  <si>
+    <t>Description 13</t>
+  </si>
+  <si>
+    <t>PopesIoon</t>
+  </si>
+  <si>
+    <t>Title 14</t>
+  </si>
+  <si>
+    <t>Description 14</t>
+  </si>
+  <si>
+    <t>PopesIooI</t>
+  </si>
+  <si>
+    <t>Title 15</t>
+  </si>
+  <si>
+    <t>Description 15</t>
+  </si>
+  <si>
+    <t>PopesIIno</t>
+  </si>
+  <si>
+    <t>Title 16</t>
+  </si>
+  <si>
+    <t>Description 16</t>
+  </si>
+  <si>
+    <t>PopesIoII</t>
+  </si>
+  <si>
+    <t>Title 17</t>
+  </si>
+  <si>
+    <t>Description 17</t>
+  </si>
+  <si>
+    <t>PopesInIn</t>
+  </si>
+  <si>
+    <t>Title 18</t>
+  </si>
+  <si>
+    <t>Description 18</t>
+  </si>
+  <si>
+    <t>PopesIIo</t>
+  </si>
+  <si>
+    <t>Title 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>PopesIon</t>
+  </si>
+  <si>
+    <t>Title 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
+  </si>
+  <si>
+    <t>PopesIono</t>
+  </si>
+  <si>
+    <t>Title 21</t>
+  </si>
+  <si>
+    <t>Description 21</t>
+  </si>
+  <si>
+    <t>PopesIIoo</t>
+  </si>
+  <si>
+    <t>Title 22</t>
+  </si>
+  <si>
+    <t>Description 22</t>
+  </si>
+  <si>
+    <t>PopesInoI</t>
+  </si>
+  <si>
+    <t>Title 23</t>
+  </si>
+  <si>
+    <t>Description 23</t>
+  </si>
+  <si>
+    <t>PopesIooIo</t>
+  </si>
+  <si>
+    <t>Title 24</t>
+  </si>
+  <si>
+    <t>Description 24</t>
+  </si>
+  <si>
+    <t>PopesIInoo</t>
+  </si>
+  <si>
+    <t>Title 25</t>
+  </si>
+  <si>
+    <t>Description 25</t>
+  </si>
+  <si>
+    <t>PopesIIon</t>
+  </si>
+  <si>
+    <t>Title 26</t>
+  </si>
+  <si>
+    <t>Description 26</t>
+  </si>
+  <si>
+    <t>PopesIoIon</t>
+  </si>
+  <si>
+    <t>Title 27</t>
+  </si>
+  <si>
+    <t>Description 27</t>
   </si>
   <si>
     <t>PopesInn</t>
   </si>
   <si>
-    <t>Title 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>a.1.5</t>
-  </si>
-  <si>
-    <t>PopesIIn</t>
-  </si>
-  <si>
-    <t>Title 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>a.1.6</t>
-  </si>
-  <si>
-    <t>PopesIII</t>
-  </si>
-  <si>
-    <t>Title 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>a.1.7</t>
-  </si>
-  <si>
-    <t>PopesIIIo</t>
-  </si>
-  <si>
-    <t>Title 8</t>
-  </si>
-  <si>
-    <t>Description 8</t>
-  </si>
-  <si>
-    <t>a.1.8</t>
-  </si>
-  <si>
-    <t>PopesIIIon</t>
-  </si>
-  <si>
-    <t>Title 9</t>
-  </si>
-  <si>
-    <t>Description 9</t>
-  </si>
-  <si>
-    <t>a.1.9</t>
-  </si>
-  <si>
-    <t>PopesIo</t>
-  </si>
-  <si>
-    <t>Title 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
-  </si>
-  <si>
-    <t>a.1.0</t>
-  </si>
-  <si>
-    <t>PopesIon</t>
-  </si>
-  <si>
-    <t>Title 11</t>
-  </si>
-  <si>
-    <t>Description 11</t>
-  </si>
-  <si>
-    <t>PopesInI</t>
-  </si>
-  <si>
-    <t>Title 12</t>
-  </si>
-  <si>
-    <t>Description 12</t>
-  </si>
-  <si>
-    <t>PopesIoI</t>
-  </si>
-  <si>
-    <t>Title 13</t>
-  </si>
-  <si>
-    <t>Description 13</t>
-  </si>
-  <si>
-    <t>PopesIoIo</t>
-  </si>
-  <si>
-    <t>Title 14</t>
-  </si>
-  <si>
-    <t>Description 14</t>
-  </si>
-  <si>
-    <t>PopesIno</t>
-  </si>
-  <si>
-    <t>Title 15</t>
-  </si>
-  <si>
-    <t>Description 15</t>
-  </si>
-  <si>
-    <t>PopesIoII</t>
-  </si>
-  <si>
-    <t>Title 16</t>
-  </si>
-  <si>
-    <t>Description 16</t>
-  </si>
-  <si>
-    <t>PopesInII</t>
-  </si>
-  <si>
-    <t>Title 17</t>
-  </si>
-  <si>
-    <t>Description 17</t>
-  </si>
-  <si>
-    <t>PopesIoIn</t>
-  </si>
-  <si>
-    <t>Title 18</t>
-  </si>
-  <si>
-    <t>Description 18</t>
-  </si>
-  <si>
-    <t>PopesInnn</t>
-  </si>
-  <si>
-    <t>Title 19</t>
-  </si>
-  <si>
-    <t>Description 19</t>
-  </si>
-  <si>
-    <t>PopesIInn</t>
-  </si>
-  <si>
-    <t>Title 20</t>
-  </si>
-  <si>
-    <t>Description 20</t>
-  </si>
-  <si>
-    <t>PopesIIIn</t>
-  </si>
-  <si>
-    <t>Title 21</t>
-  </si>
-  <si>
-    <t>Description 21</t>
-  </si>
-  <si>
-    <t>PopesIono</t>
-  </si>
-  <si>
-    <t>Title 22</t>
-  </si>
-  <si>
-    <t>Description 22</t>
-  </si>
-  <si>
-    <t>PopesInoI</t>
-  </si>
-  <si>
-    <t>Title 23</t>
-  </si>
-  <si>
-    <t>Description 23</t>
-  </si>
-  <si>
-    <t>PopesIoIoI</t>
-  </si>
-  <si>
-    <t>Title 24</t>
-  </si>
-  <si>
-    <t>Description 24</t>
-  </si>
-  <si>
-    <t>PopesInIIn</t>
-  </si>
-  <si>
-    <t>Title 25</t>
-  </si>
-  <si>
-    <t>Description 25</t>
-  </si>
-  <si>
-    <t>PopesInIn</t>
-  </si>
-  <si>
-    <t>Title 26</t>
-  </si>
-  <si>
-    <t>Description 26</t>
-  </si>
-  <si>
-    <t>PopesIIII</t>
-  </si>
-  <si>
-    <t>Title 27</t>
-  </si>
-  <si>
-    <t>Description 27</t>
-  </si>
-  <si>
-    <t>PopesIoo</t>
-  </si>
-  <si>
     <t>Title 28</t>
   </si>
   <si>
     <t>Description 28</t>
   </si>
   <si>
-    <t>PopesInno</t>
+    <t>PopesInIno</t>
   </si>
   <si>
     <t>Title 29</t>
@@ -353,7 +353,7 @@
     <t>Description 29</t>
   </si>
   <si>
-    <t>PopesInnI</t>
+    <t>PopesInInoI</t>
   </si>
   <si>
     <t>Title 30</t>
@@ -362,7 +362,7 @@
     <t>Description 30</t>
   </si>
   <si>
-    <t>PopesIooI</t>
+    <t>PopesIIoI</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" t="n" s="2">
-        <v>43321.656944375</v>
+        <v>43321.68707503472</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -519,7 +519,7 @@
       </c>
       <c r="E3"/>
       <c r="F3" t="n" s="2">
-        <v>43321.656944675924</v>
+        <v>43321.68707539352</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -552,7 +552,7 @@
       </c>
       <c r="E4"/>
       <c r="F4" t="n" s="2">
-        <v>43321.65694497685</v>
+        <v>43321.687075752314</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -585,7 +585,7 @@
       </c>
       <c r="E5"/>
       <c r="F5" t="n" s="2">
-        <v>43321.656945104165</v>
+        <v>43321.6870759375</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -618,19 +618,19 @@
       </c>
       <c r="E6"/>
       <c r="F6" t="n" s="2">
-        <v>43321.65694527778</v>
+        <v>43321.68707612268</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
         <v>18</v>
@@ -651,7 +651,7 @@
       </c>
       <c r="E7"/>
       <c r="F7" t="n" s="2">
-        <v>43321.65694547454</v>
+        <v>43321.68707629629</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -684,7 +684,7 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n" s="2">
-        <v>43321.65694565972</v>
+        <v>43321.68707648148</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
@@ -717,7 +717,7 @@
       </c>
       <c r="E9"/>
       <c r="F9" t="n" s="2">
-        <v>43321.65694586805</v>
+        <v>43321.68707666667</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
@@ -750,7 +750,7 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n" s="2">
-        <v>43321.65694608796</v>
+        <v>43321.68707684028</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -783,7 +783,7 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n" s="2">
-        <v>43321.65694622685</v>
+        <v>43321.68707702546</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
@@ -816,19 +816,19 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n" s="2">
-        <v>43321.656946400464</v>
+        <v>43321.68707702546</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s">
         <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
         <v>18</v>
@@ -849,19 +849,19 @@
       </c>
       <c r="E13"/>
       <c r="F13" t="n" s="2">
-        <v>43321.65694659722</v>
+        <v>43321.68707719907</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
@@ -882,7 +882,7 @@
       </c>
       <c r="E14"/>
       <c r="F14" t="n" s="2">
-        <v>43321.656946759256</v>
+        <v>43321.68707738426</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="E15"/>
       <c r="F15" t="n" s="2">
-        <v>43321.656946967596</v>
+        <v>43321.68707756945</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
@@ -948,19 +948,19 @@
       </c>
       <c r="E16"/>
       <c r="F16" t="n" s="2">
-        <v>43321.65694712963</v>
+        <v>43321.68707774305</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
         <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
         <v>18</v>
@@ -981,19 +981,19 @@
       </c>
       <c r="E17"/>
       <c r="F17" t="n" s="2">
-        <v>43321.65694729167</v>
+        <v>43321.68707792824</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H17" t="s">
         <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K17" t="s">
         <v>18</v>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="E18"/>
       <c r="F18" t="n" s="2">
-        <v>43321.65694746528</v>
+        <v>43321.68707811343</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -1047,19 +1047,19 @@
       </c>
       <c r="E19"/>
       <c r="F19" t="n" s="2">
-        <v>43321.656947627314</v>
+        <v>43321.68707828704</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -1080,19 +1080,19 @@
       </c>
       <c r="E20"/>
       <c r="F20" t="n" s="2">
-        <v>43321.65694777778</v>
+        <v>43321.68707847222</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
         <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="J20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
@@ -1113,19 +1113,19 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n" s="2">
-        <v>43321.65694793982</v>
+        <v>43321.68707864583</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H21" t="s">
         <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
@@ -1146,19 +1146,19 @@
       </c>
       <c r="E22"/>
       <c r="F22" t="n" s="2">
-        <v>43321.65694811343</v>
+        <v>43321.68707883102</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s">
         <v>89</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E23"/>
       <c r="F23" t="n" s="2">
-        <v>43321.65694825231</v>
+        <v>43321.68707901621</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="E24"/>
       <c r="F24" t="n" s="2">
-        <v>43321.65694849537</v>
+        <v>43321.68707918982</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E25"/>
       <c r="F25" t="n" s="2">
-        <v>43321.656948703705</v>
+        <v>43321.687079375</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -1278,19 +1278,19 @@
       </c>
       <c r="E26"/>
       <c r="F26" t="n" s="2">
-        <v>43321.656948888885</v>
+        <v>43321.687079560186</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H26" t="s">
         <v>101</v>
       </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="E27"/>
       <c r="F27" t="n" s="2">
-        <v>43321.65694903935</v>
+        <v>43321.6870797338</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E28"/>
       <c r="F28" t="n" s="2">
-        <v>43321.65694920139</v>
+        <v>43321.68707991898</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
@@ -1377,19 +1377,19 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n" s="2">
-        <v>43321.6569493287</v>
+        <v>43321.68708009259</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H29" t="s">
         <v>110</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n" s="2">
-        <v>43321.65694949074</v>
+        <v>43321.68708027778</v>
       </c>
       <c r="G30" t="s">
         <v>22</v>
@@ -1443,19 +1443,19 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n" s="2">
-        <v>43321.656949641205</v>
+        <v>43321.687080462965</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H31" t="s">
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
modified styles.css and edit user datatable
</commit_message>
<xml_diff>
--- a/ExcelBugs.xlsx
+++ b/ExcelBugs.xlsx
@@ -56,10 +56,79 @@
     <t>a.1.1</t>
   </si>
   <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>PopesI</t>
+  </si>
+  <si>
+    <t>IN_PROGRESS</t>
+  </si>
+  <si>
+    <t>BUG_STATUS_UPDATED</t>
+  </si>
+  <si>
+    <t>Title 2</t>
+  </si>
+  <si>
+    <t>Description 2</t>
+  </si>
+  <si>
+    <t>a.1.2</t>
+  </si>
+  <si>
+    <t>PopesIn</t>
+  </si>
+  <si>
+    <t>Title 3</t>
+  </si>
+  <si>
+    <t>Description 3</t>
+  </si>
+  <si>
+    <t>a.1.3</t>
+  </si>
+  <si>
+    <t>PopesIo</t>
+  </si>
+  <si>
+    <t>Title 4</t>
+  </si>
+  <si>
+    <t>Description 4</t>
+  </si>
+  <si>
+    <t>a.1.4</t>
+  </si>
+  <si>
+    <t>PopesIoI</t>
+  </si>
+  <si>
+    <t>Title 5</t>
+  </si>
+  <si>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>a.1.5</t>
+  </si>
+  <si>
+    <t>PopesInn</t>
+  </si>
+  <si>
+    <t>Title 6</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>a.1.6</t>
+  </si>
+  <si>
     <t>LOW</t>
   </si>
   <si>
-    <t>PopesI</t>
+    <t>PopesIoo</t>
   </si>
   <si>
     <t>Nobody</t>
@@ -68,301 +137,232 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>BUG_STATUS_UPDATED</t>
-  </si>
-  <si>
-    <t>Title 2</t>
-  </si>
-  <si>
-    <t>Description 2</t>
-  </si>
-  <si>
-    <t>a.1.2</t>
-  </si>
-  <si>
-    <t>CRITICAL</t>
+    <t>Title 7</t>
+  </si>
+  <si>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>a.1.7</t>
+  </si>
+  <si>
+    <t>PopesIoII</t>
+  </si>
+  <si>
+    <t>Title 8</t>
+  </si>
+  <si>
+    <t>Description 8</t>
+  </si>
+  <si>
+    <t>a.1.8</t>
+  </si>
+  <si>
+    <t>PopesIoIII</t>
+  </si>
+  <si>
+    <t>Title 9</t>
+  </si>
+  <si>
+    <t>Description 9</t>
+  </si>
+  <si>
+    <t>a.1.9</t>
+  </si>
+  <si>
+    <t>PopesInI</t>
+  </si>
+  <si>
+    <t>Title 10</t>
+  </si>
+  <si>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>a.1.0</t>
   </si>
   <si>
     <t>PopesII</t>
   </si>
   <si>
-    <t>IN_PROGRESS</t>
-  </si>
-  <si>
-    <t>Title 3</t>
-  </si>
-  <si>
-    <t>Description 3</t>
-  </si>
-  <si>
-    <t>a.1.3</t>
-  </si>
-  <si>
-    <t>PopesIn</t>
-  </si>
-  <si>
-    <t>Title 4</t>
-  </si>
-  <si>
-    <t>Description 4</t>
-  </si>
-  <si>
-    <t>a.1.4</t>
-  </si>
-  <si>
-    <t>PopesIo</t>
-  </si>
-  <si>
-    <t>Title 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>a.1.5</t>
-  </si>
-  <si>
-    <t>PopesIIn</t>
-  </si>
-  <si>
-    <t>Title 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>a.1.6</t>
-  </si>
-  <si>
-    <t>PopesInn</t>
-  </si>
-  <si>
-    <t>Title 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>a.1.7</t>
-  </si>
-  <si>
-    <t>PopesIoI</t>
-  </si>
-  <si>
-    <t>Title 8</t>
-  </si>
-  <si>
-    <t>Description 8</t>
-  </si>
-  <si>
-    <t>a.1.8</t>
+    <t>Title 11</t>
+  </si>
+  <si>
+    <t>Description 11</t>
+  </si>
+  <si>
+    <t>PopesIon</t>
+  </si>
+  <si>
+    <t>Title 12</t>
+  </si>
+  <si>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>PopesInIn</t>
+  </si>
+  <si>
+    <t>Title 13</t>
+  </si>
+  <si>
+    <t>Description 13</t>
+  </si>
+  <si>
+    <t>PopesIno</t>
+  </si>
+  <si>
+    <t>Title 14</t>
+  </si>
+  <si>
+    <t>Description 14</t>
+  </si>
+  <si>
+    <t>PopesInno</t>
+  </si>
+  <si>
+    <t>Title 15</t>
+  </si>
+  <si>
+    <t>Description 15</t>
+  </si>
+  <si>
+    <t>PopesInon</t>
+  </si>
+  <si>
+    <t>Title 16</t>
+  </si>
+  <si>
+    <t>Description 16</t>
+  </si>
+  <si>
+    <t>PopesIIo</t>
+  </si>
+  <si>
+    <t>Title 17</t>
+  </si>
+  <si>
+    <t>Description 17</t>
+  </si>
+  <si>
+    <t>PopesInInI</t>
+  </si>
+  <si>
+    <t>Title 18</t>
+  </si>
+  <si>
+    <t>Description 18</t>
+  </si>
+  <si>
+    <t>PopesIonn</t>
+  </si>
+  <si>
+    <t>Title 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>PopesInIo</t>
+  </si>
+  <si>
+    <t>Title 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
+  </si>
+  <si>
+    <t>PopesInonI</t>
+  </si>
+  <si>
+    <t>Title 21</t>
+  </si>
+  <si>
+    <t>Description 21</t>
+  </si>
+  <si>
+    <t>PopesIIoo</t>
+  </si>
+  <si>
+    <t>Title 22</t>
+  </si>
+  <si>
+    <t>Description 22</t>
+  </si>
+  <si>
+    <t>PopesIonnn</t>
+  </si>
+  <si>
+    <t>Title 23</t>
+  </si>
+  <si>
+    <t>Description 23</t>
+  </si>
+  <si>
+    <t>PopesIoon</t>
+  </si>
+  <si>
+    <t>Title 24</t>
+  </si>
+  <si>
+    <t>Description 24</t>
   </si>
   <si>
     <t>PopesIII</t>
   </si>
   <si>
-    <t>Title 9</t>
-  </si>
-  <si>
-    <t>Description 9</t>
-  </si>
-  <si>
-    <t>a.1.9</t>
-  </si>
-  <si>
-    <t>PopesInnI</t>
-  </si>
-  <si>
-    <t>Title 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
-  </si>
-  <si>
-    <t>a.1.0</t>
-  </si>
-  <si>
-    <t>PopesIInn</t>
-  </si>
-  <si>
-    <t>Title 11</t>
-  </si>
-  <si>
-    <t>Description 11</t>
+    <t>Title 25</t>
+  </si>
+  <si>
+    <t>Description 25</t>
+  </si>
+  <si>
+    <t>PopesIoonn</t>
+  </si>
+  <si>
+    <t>Title 26</t>
+  </si>
+  <si>
+    <t>Description 26</t>
+  </si>
+  <si>
+    <t>PopesInIoI</t>
+  </si>
+  <si>
+    <t>Title 27</t>
+  </si>
+  <si>
+    <t>Description 27</t>
+  </si>
+  <si>
+    <t>PopesIIoI</t>
+  </si>
+  <si>
+    <t>Title 28</t>
+  </si>
+  <si>
+    <t>Description 28</t>
+  </si>
+  <si>
+    <t>PopesIono</t>
+  </si>
+  <si>
+    <t>Title 29</t>
+  </si>
+  <si>
+    <t>Description 29</t>
   </si>
   <si>
     <t>PopesIoIn</t>
   </si>
   <si>
-    <t>Title 12</t>
-  </si>
-  <si>
-    <t>Description 12</t>
-  </si>
-  <si>
-    <t>PopesIIo</t>
-  </si>
-  <si>
-    <t>Title 13</t>
-  </si>
-  <si>
-    <t>Description 13</t>
-  </si>
-  <si>
-    <t>PopesIIno</t>
-  </si>
-  <si>
-    <t>Title 14</t>
-  </si>
-  <si>
-    <t>Description 14</t>
-  </si>
-  <si>
-    <t>PopesIIIo</t>
-  </si>
-  <si>
-    <t>Title 15</t>
-  </si>
-  <si>
-    <t>Description 15</t>
-  </si>
-  <si>
-    <t>PopesIno</t>
-  </si>
-  <si>
-    <t>Title 16</t>
-  </si>
-  <si>
-    <t>Description 16</t>
-  </si>
-  <si>
-    <t>PopesIInnI</t>
-  </si>
-  <si>
-    <t>Title 17</t>
-  </si>
-  <si>
-    <t>Description 17</t>
-  </si>
-  <si>
-    <t>PopesIIIoI</t>
-  </si>
-  <si>
-    <t>Title 18</t>
-  </si>
-  <si>
-    <t>Description 18</t>
-  </si>
-  <si>
-    <t>PopesIon</t>
-  </si>
-  <si>
-    <t>Title 19</t>
-  </si>
-  <si>
-    <t>Description 19</t>
-  </si>
-  <si>
-    <t>PopesInnn</t>
-  </si>
-  <si>
-    <t>Title 20</t>
-  </si>
-  <si>
-    <t>Description 20</t>
-  </si>
-  <si>
-    <t>PopesIIoI</t>
-  </si>
-  <si>
-    <t>Title 21</t>
-  </si>
-  <si>
-    <t>Description 21</t>
-  </si>
-  <si>
-    <t>PopesIono</t>
-  </si>
-  <si>
-    <t>Title 22</t>
-  </si>
-  <si>
-    <t>Description 22</t>
-  </si>
-  <si>
-    <t>PopesIoo</t>
-  </si>
-  <si>
-    <t>Title 23</t>
-  </si>
-  <si>
-    <t>Description 23</t>
-  </si>
-  <si>
-    <t>PopesIIIn</t>
-  </si>
-  <si>
-    <t>Title 24</t>
-  </si>
-  <si>
-    <t>Description 24</t>
-  </si>
-  <si>
-    <t>PopesIIInn</t>
-  </si>
-  <si>
-    <t>Title 25</t>
-  </si>
-  <si>
-    <t>Description 25</t>
-  </si>
-  <si>
-    <t>PopesInoo</t>
-  </si>
-  <si>
-    <t>Title 26</t>
-  </si>
-  <si>
-    <t>Description 26</t>
-  </si>
-  <si>
-    <t>PopesInI</t>
-  </si>
-  <si>
-    <t>Title 27</t>
-  </si>
-  <si>
-    <t>Description 27</t>
-  </si>
-  <si>
-    <t>PopesIoIo</t>
-  </si>
-  <si>
-    <t>Title 28</t>
-  </si>
-  <si>
-    <t>Description 28</t>
-  </si>
-  <si>
-    <t>PopesInno</t>
-  </si>
-  <si>
-    <t>Title 29</t>
-  </si>
-  <si>
-    <t>Description 29</t>
-  </si>
-  <si>
-    <t>PopesIoInn</t>
-  </si>
-  <si>
     <t>Title 30</t>
   </si>
   <si>
     <t>Description 30</t>
   </si>
   <si>
-    <t>PopesInIo</t>
+    <t>PopesIonoI</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" t="n" s="2">
-        <v>43322.644175277776</v>
+        <v>43325.42435291666</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -495,13 +495,13 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -509,32 +509,32 @@
         <v>16.0</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="n" s="2">
-        <v>43322.644175636575</v>
+        <v>43325.42435327546</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -542,32 +542,32 @@
         <v>25.0</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4"/>
       <c r="F4" t="n" s="2">
-        <v>43322.64417599537</v>
+        <v>43325.424353449074</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -575,32 +575,32 @@
         <v>34.0</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="n" s="2">
-        <v>43322.64417599537</v>
+        <v>43325.42435363426</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -608,32 +608,32 @@
         <v>43.0</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="n" s="2">
-        <v>43322.644176180554</v>
+        <v>43325.424353993054</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -641,32 +641,32 @@
         <v>52.0</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="n" s="2">
-        <v>43322.64417636574</v>
+        <v>43325.42435417824</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -684,22 +684,22 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n" s="2">
-        <v>43322.644176724534</v>
+        <v>43325.42435436343</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -717,22 +717,22 @@
       </c>
       <c r="E9"/>
       <c r="F9" t="n" s="2">
-        <v>43322.644176898146</v>
+        <v>43325.424354537034</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -750,10 +750,10 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n" s="2">
-        <v>43322.64417708333</v>
+        <v>43325.42435508102</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
         <v>52</v>
@@ -762,10 +762,10 @@
         <v>52</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -783,22 +783,22 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n" s="2">
-        <v>43322.64417726852</v>
+        <v>43325.4243552662</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -816,7 +816,7 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n" s="2">
-        <v>43322.64417744213</v>
+        <v>43325.42435543981</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -825,13 +825,13 @@
         <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -845,26 +845,26 @@
         <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13"/>
       <c r="F13" t="n" s="2">
-        <v>43322.64417762731</v>
+        <v>43325.42435581019</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -878,14 +878,14 @@
         <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14"/>
       <c r="F14" t="n" s="2">
-        <v>43322.6441778125</v>
+        <v>43325.4243559838</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>65</v>
@@ -894,10 +894,10 @@
         <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -911,26 +911,26 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="n" s="2">
-        <v>43322.64417798611</v>
+        <v>43325.42435634259</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H15" t="s">
         <v>68</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -944,11 +944,11 @@
         <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="n" s="2">
-        <v>43322.64417817129</v>
+        <v>43325.42435652778</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -957,13 +957,13 @@
         <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -977,11 +977,11 @@
         <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="n" s="2">
-        <v>43322.644178344905</v>
+        <v>43325.42435671296</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
@@ -990,13 +990,13 @@
         <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1014,10 +1014,10 @@
       </c>
       <c r="E18"/>
       <c r="F18" t="n" s="2">
-        <v>43322.64417853009</v>
+        <v>43325.42435688657</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
         <v>77</v>
@@ -1026,10 +1026,10 @@
         <v>77</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="E19"/>
       <c r="F19" t="n" s="2">
-        <v>43322.64417871528</v>
+        <v>43325.42435707176</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1056,13 +1056,13 @@
         <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -1080,10 +1080,10 @@
       </c>
       <c r="E20"/>
       <c r="F20" t="n" s="2">
-        <v>43322.64417888889</v>
+        <v>43325.42435743056</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
         <v>83</v>
@@ -1092,10 +1092,10 @@
         <v>83</v>
       </c>
       <c r="J20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -1113,22 +1113,22 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n" s="2">
-        <v>43322.64417907407</v>
+        <v>43325.42435761574</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H21" t="s">
         <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="K21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
@@ -1146,10 +1146,10 @@
       </c>
       <c r="E22"/>
       <c r="F22" t="n" s="2">
-        <v>43322.64417925926</v>
+        <v>43325.42435797454</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
         <v>89</v>
@@ -1158,10 +1158,10 @@
         <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
@@ -1175,14 +1175,14 @@
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23"/>
       <c r="F23" t="n" s="2">
-        <v>43322.64417943287</v>
+        <v>43325.424358159726</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s">
         <v>92</v>
@@ -1191,10 +1191,10 @@
         <v>92</v>
       </c>
       <c r="J23" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
@@ -1208,26 +1208,26 @@
         <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E24"/>
       <c r="F24" t="n" s="2">
-        <v>43322.64417961806</v>
+        <v>43325.42435833333</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H24" t="s">
         <v>95</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -1241,14 +1241,14 @@
         <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E25"/>
       <c r="F25" t="n" s="2">
-        <v>43322.64417979166</v>
+        <v>43325.424358703705</v>
       </c>
       <c r="G25" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
         <v>98</v>
@@ -1257,10 +1257,10 @@
         <v>98</v>
       </c>
       <c r="J25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
@@ -1274,26 +1274,26 @@
         <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E26"/>
       <c r="F26" t="n" s="2">
-        <v>43322.64417997685</v>
+        <v>43325.42435887732</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H26" t="s">
         <v>101</v>
       </c>
       <c r="I26" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
@@ -1307,26 +1307,26 @@
         <v>103</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E27"/>
       <c r="F27" t="n" s="2">
-        <v>43322.64418016204</v>
+        <v>43325.4243590625</v>
       </c>
       <c r="G27" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H27" t="s">
         <v>104</v>
       </c>
       <c r="I27" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="J27" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
@@ -1344,10 +1344,10 @@
       </c>
       <c r="E28"/>
       <c r="F28" t="n" s="2">
-        <v>43322.64418033565</v>
+        <v>43325.4243594213</v>
       </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
         <v>107</v>
@@ -1356,10 +1356,10 @@
         <v>107</v>
       </c>
       <c r="J28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
@@ -1377,22 +1377,22 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n" s="2">
-        <v>43322.64418052083</v>
+        <v>43325.424359606484</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H29" t="s">
         <v>110</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="K29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
@@ -1410,22 +1410,22 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n" s="2">
-        <v>43322.64418087963</v>
+        <v>43325.42435996528</v>
       </c>
       <c r="G30" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H30" t="s">
         <v>113</v>
       </c>
       <c r="I30" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="J30" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n" s="2">
-        <v>43322.64418106482</v>
+        <v>43325.424360150464</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
@@ -1452,13 +1452,13 @@
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge with master and format
</commit_message>
<xml_diff>
--- a/ExcelBugs.xlsx
+++ b/ExcelBugs.xlsx
@@ -56,42 +56,51 @@
     <t>a.1.1</t>
   </si>
   <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>PopesI</t>
+  </si>
+  <si>
+    <t>Nobody</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>BUG_STATUS_UPDATED</t>
+  </si>
+  <si>
+    <t>Title 2</t>
+  </si>
+  <si>
+    <t>Description 2</t>
+  </si>
+  <si>
+    <t>a.1.2</t>
+  </si>
+  <si>
+    <t>PopesIn</t>
+  </si>
+  <si>
+    <t>Title 3</t>
+  </si>
+  <si>
+    <t>Description 3</t>
+  </si>
+  <si>
+    <t>a.1.3</t>
+  </si>
+  <si>
     <t>CRITICAL</t>
   </si>
   <si>
-    <t>PopesI</t>
+    <t>PopesIo</t>
   </si>
   <si>
     <t>IN_PROGRESS</t>
   </si>
   <si>
-    <t>BUG_STATUS_UPDATED</t>
-  </si>
-  <si>
-    <t>Title 2</t>
-  </si>
-  <si>
-    <t>Description 2</t>
-  </si>
-  <si>
-    <t>a.1.2</t>
-  </si>
-  <si>
-    <t>PopesIn</t>
-  </si>
-  <si>
-    <t>Title 3</t>
-  </si>
-  <si>
-    <t>Description 3</t>
-  </si>
-  <si>
-    <t>a.1.3</t>
-  </si>
-  <si>
-    <t>PopesIo</t>
-  </si>
-  <si>
     <t>Title 4</t>
   </si>
   <si>
@@ -101,241 +110,232 @@
     <t>a.1.4</t>
   </si>
   <si>
+    <t>PopesII</t>
+  </si>
+  <si>
+    <t>Title 5</t>
+  </si>
+  <si>
+    <t>Description 5</t>
+  </si>
+  <si>
+    <t>a.1.5</t>
+  </si>
+  <si>
+    <t>PopesIIn</t>
+  </si>
+  <si>
+    <t>Title 6</t>
+  </si>
+  <si>
+    <t>Description 6</t>
+  </si>
+  <si>
+    <t>a.1.6</t>
+  </si>
+  <si>
+    <t>PopesIInn</t>
+  </si>
+  <si>
+    <t>Title 7</t>
+  </si>
+  <si>
+    <t>Description 7</t>
+  </si>
+  <si>
+    <t>a.1.7</t>
+  </si>
+  <si>
     <t>PopesIoI</t>
   </si>
   <si>
-    <t>Title 5</t>
-  </si>
-  <si>
-    <t>Description 5</t>
-  </si>
-  <si>
-    <t>a.1.5</t>
+    <t>Title 8</t>
+  </si>
+  <si>
+    <t>Description 8</t>
+  </si>
+  <si>
+    <t>a.1.8</t>
+  </si>
+  <si>
+    <t>PopesIII</t>
+  </si>
+  <si>
+    <t>Title 9</t>
+  </si>
+  <si>
+    <t>Description 9</t>
+  </si>
+  <si>
+    <t>a.1.9</t>
+  </si>
+  <si>
+    <t>PopesIoIo</t>
+  </si>
+  <si>
+    <t>Title 10</t>
+  </si>
+  <si>
+    <t>Description 10</t>
+  </si>
+  <si>
+    <t>a.1.0</t>
+  </si>
+  <si>
+    <t>PopesIon</t>
+  </si>
+  <si>
+    <t>Title 11</t>
+  </si>
+  <si>
+    <t>Description 11</t>
+  </si>
+  <si>
+    <t>PopesIonI</t>
+  </si>
+  <si>
+    <t>Title 12</t>
+  </si>
+  <si>
+    <t>Description 12</t>
+  </si>
+  <si>
+    <t>PopesInI</t>
+  </si>
+  <si>
+    <t>Title 13</t>
+  </si>
+  <si>
+    <t>Description 13</t>
+  </si>
+  <si>
+    <t>PopesIInnI</t>
+  </si>
+  <si>
+    <t>Title 14</t>
+  </si>
+  <si>
+    <t>Description 14</t>
+  </si>
+  <si>
+    <t>PopesIonn</t>
+  </si>
+  <si>
+    <t>Title 15</t>
+  </si>
+  <si>
+    <t>Description 15</t>
+  </si>
+  <si>
+    <t>PopesIonnI</t>
+  </si>
+  <si>
+    <t>Title 16</t>
+  </si>
+  <si>
+    <t>Description 16</t>
+  </si>
+  <si>
+    <t>PopesIno</t>
+  </si>
+  <si>
+    <t>Title 17</t>
+  </si>
+  <si>
+    <t>Description 17</t>
   </si>
   <si>
     <t>PopesInn</t>
   </si>
   <si>
-    <t>Title 6</t>
-  </si>
-  <si>
-    <t>Description 6</t>
-  </si>
-  <si>
-    <t>a.1.6</t>
-  </si>
-  <si>
-    <t>LOW</t>
+    <t>Title 18</t>
+  </si>
+  <si>
+    <t>Description 18</t>
+  </si>
+  <si>
+    <t>PopesInoo</t>
+  </si>
+  <si>
+    <t>Title 19</t>
+  </si>
+  <si>
+    <t>Description 19</t>
+  </si>
+  <si>
+    <t>PopesIIII</t>
+  </si>
+  <si>
+    <t>Title 20</t>
+  </si>
+  <si>
+    <t>Description 20</t>
   </si>
   <si>
     <t>PopesIoo</t>
   </si>
   <si>
-    <t>Nobody</t>
-  </si>
-  <si>
-    <t>NEW</t>
-  </si>
-  <si>
-    <t>Title 7</t>
-  </si>
-  <si>
-    <t>Description 7</t>
-  </si>
-  <si>
-    <t>a.1.7</t>
-  </si>
-  <si>
-    <t>PopesIoII</t>
-  </si>
-  <si>
-    <t>Title 8</t>
-  </si>
-  <si>
-    <t>Description 8</t>
-  </si>
-  <si>
-    <t>a.1.8</t>
-  </si>
-  <si>
-    <t>PopesIoIII</t>
-  </si>
-  <si>
-    <t>Title 9</t>
-  </si>
-  <si>
-    <t>Description 9</t>
-  </si>
-  <si>
-    <t>a.1.9</t>
-  </si>
-  <si>
-    <t>PopesInI</t>
-  </si>
-  <si>
-    <t>Title 10</t>
-  </si>
-  <si>
-    <t>Description 10</t>
-  </si>
-  <si>
-    <t>a.1.0</t>
-  </si>
-  <si>
-    <t>PopesII</t>
-  </si>
-  <si>
-    <t>Title 11</t>
-  </si>
-  <si>
-    <t>Description 11</t>
-  </si>
-  <si>
-    <t>PopesIon</t>
-  </si>
-  <si>
-    <t>Title 12</t>
-  </si>
-  <si>
-    <t>Description 12</t>
-  </si>
-  <si>
-    <t>PopesInIn</t>
-  </si>
-  <si>
-    <t>Title 13</t>
-  </si>
-  <si>
-    <t>Description 13</t>
-  </si>
-  <si>
-    <t>PopesIno</t>
-  </si>
-  <si>
-    <t>Title 14</t>
-  </si>
-  <si>
-    <t>Description 14</t>
-  </si>
-  <si>
-    <t>PopesInno</t>
-  </si>
-  <si>
-    <t>Title 15</t>
-  </si>
-  <si>
-    <t>Description 15</t>
-  </si>
-  <si>
-    <t>PopesInon</t>
-  </si>
-  <si>
-    <t>Title 16</t>
-  </si>
-  <si>
-    <t>Description 16</t>
+    <t>Title 21</t>
+  </si>
+  <si>
+    <t>Description 21</t>
+  </si>
+  <si>
+    <t>PopesInooo</t>
+  </si>
+  <si>
+    <t>Title 22</t>
+  </si>
+  <si>
+    <t>Description 22</t>
+  </si>
+  <si>
+    <t>PopesIoon</t>
+  </si>
+  <si>
+    <t>Title 23</t>
+  </si>
+  <si>
+    <t>Description 23</t>
+  </si>
+  <si>
+    <t>PopesIonnn</t>
+  </si>
+  <si>
+    <t>Title 24</t>
+  </si>
+  <si>
+    <t>Description 24</t>
   </si>
   <si>
     <t>PopesIIo</t>
   </si>
   <si>
-    <t>Title 17</t>
-  </si>
-  <si>
-    <t>Description 17</t>
-  </si>
-  <si>
-    <t>PopesInInI</t>
-  </si>
-  <si>
-    <t>Title 18</t>
-  </si>
-  <si>
-    <t>Description 18</t>
-  </si>
-  <si>
-    <t>PopesIonn</t>
-  </si>
-  <si>
-    <t>Title 19</t>
-  </si>
-  <si>
-    <t>Description 19</t>
-  </si>
-  <si>
-    <t>PopesInIo</t>
-  </si>
-  <si>
-    <t>Title 20</t>
-  </si>
-  <si>
-    <t>Description 20</t>
-  </si>
-  <si>
-    <t>PopesInonI</t>
-  </si>
-  <si>
-    <t>Title 21</t>
-  </si>
-  <si>
-    <t>Description 21</t>
+    <t>Title 25</t>
+  </si>
+  <si>
+    <t>Description 25</t>
+  </si>
+  <si>
+    <t>PopesIoIoI</t>
+  </si>
+  <si>
+    <t>Title 26</t>
+  </si>
+  <si>
+    <t>Description 26</t>
   </si>
   <si>
     <t>PopesIIoo</t>
   </si>
   <si>
-    <t>Title 22</t>
-  </si>
-  <si>
-    <t>Description 22</t>
-  </si>
-  <si>
-    <t>PopesIonnn</t>
-  </si>
-  <si>
-    <t>Title 23</t>
-  </si>
-  <si>
-    <t>Description 23</t>
-  </si>
-  <si>
-    <t>PopesIoon</t>
-  </si>
-  <si>
-    <t>Title 24</t>
-  </si>
-  <si>
-    <t>Description 24</t>
-  </si>
-  <si>
-    <t>PopesIII</t>
-  </si>
-  <si>
-    <t>Title 25</t>
-  </si>
-  <si>
-    <t>Description 25</t>
-  </si>
-  <si>
-    <t>PopesIoonn</t>
-  </si>
-  <si>
-    <t>Title 26</t>
-  </si>
-  <si>
-    <t>Description 26</t>
-  </si>
-  <si>
-    <t>PopesInIoI</t>
-  </si>
-  <si>
     <t>Title 27</t>
   </si>
   <si>
     <t>Description 27</t>
   </si>
   <si>
-    <t>PopesIIoI</t>
+    <t>PopesInnn</t>
   </si>
   <si>
     <t>Title 28</t>
@@ -344,7 +344,7 @@
     <t>Description 28</t>
   </si>
   <si>
-    <t>PopesIono</t>
+    <t>PopesIoIn</t>
   </si>
   <si>
     <t>Title 29</t>
@@ -353,7 +353,7 @@
     <t>Description 29</t>
   </si>
   <si>
-    <t>PopesIoIn</t>
+    <t>PopesIonnno</t>
   </si>
   <si>
     <t>Title 30</t>
@@ -362,7 +362,7 @@
     <t>Description 30</t>
   </si>
   <si>
-    <t>PopesIonoI</t>
+    <t>PopesIInnIn</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" t="n" s="2">
-        <v>43325.42435291666</v>
+        <v>43328.6624855787</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -495,13 +495,13 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -509,32 +509,32 @@
         <v>16.0</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="n" s="2">
-        <v>43325.42435327546</v>
+        <v>43328.6624859375</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -542,32 +542,32 @@
         <v>25.0</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4"/>
       <c r="F4" t="n" s="2">
-        <v>43325.424353449074</v>
+        <v>43328.66248612269</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -575,32 +575,32 @@
         <v>34.0</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="n" s="2">
-        <v>43325.42435363426</v>
+        <v>43328.6624862963</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -608,32 +608,32 @@
         <v>43.0</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="n" s="2">
-        <v>43325.424353993054</v>
+        <v>43328.66248648148</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -641,32 +641,32 @@
         <v>52.0</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="n" s="2">
-        <v>43325.42435417824</v>
+        <v>43328.66248665509</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -684,22 +684,22 @@
       </c>
       <c r="E8"/>
       <c r="F8" t="n" s="2">
-        <v>43325.42435436343</v>
+        <v>43328.66248702546</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -717,22 +717,22 @@
       </c>
       <c r="E9"/>
       <c r="F9" t="n" s="2">
-        <v>43325.424354537034</v>
+        <v>43328.66248719907</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -750,7 +750,7 @@
       </c>
       <c r="E10"/>
       <c r="F10" t="n" s="2">
-        <v>43325.42435508102</v>
+        <v>43328.66248756945</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -759,13 +759,13 @@
         <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -783,22 +783,22 @@
       </c>
       <c r="E11"/>
       <c r="F11" t="n" s="2">
-        <v>43325.4243552662</v>
+        <v>43328.66248774306</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>56</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -816,7 +816,7 @@
       </c>
       <c r="E12"/>
       <c r="F12" t="n" s="2">
-        <v>43325.42435543981</v>
+        <v>43328.66248792824</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -825,13 +825,13 @@
         <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -845,26 +845,26 @@
         <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13"/>
       <c r="F13" t="n" s="2">
-        <v>43325.42435581019</v>
+        <v>43328.66248810185</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -878,14 +878,14 @@
         <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14"/>
       <c r="F14" t="n" s="2">
-        <v>43325.4243559838</v>
+        <v>43328.66248828704</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H14" t="s">
         <v>65</v>
@@ -894,10 +894,10 @@
         <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
@@ -911,26 +911,26 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="n" s="2">
-        <v>43325.42435634259</v>
+        <v>43328.66248847222</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H15" t="s">
         <v>68</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="J15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
@@ -944,14 +944,14 @@
         <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="n" s="2">
-        <v>43325.42435652778</v>
+        <v>43328.66248883102</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H16" t="s">
         <v>71</v>
@@ -960,10 +960,10 @@
         <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17">
@@ -977,14 +977,14 @@
         <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="n" s="2">
-        <v>43325.42435671296</v>
+        <v>43328.662489016206</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H17" t="s">
         <v>74</v>
@@ -993,10 +993,10 @@
         <v>74</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="E18"/>
       <c r="F18" t="n" s="2">
-        <v>43325.42435688657</v>
+        <v>43328.66248918982</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
@@ -1023,13 +1023,13 @@
         <v>77</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="E19"/>
       <c r="F19" t="n" s="2">
-        <v>43325.42435707176</v>
+        <v>43328.662489375</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1056,13 +1056,13 @@
         <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -1080,10 +1080,10 @@
       </c>
       <c r="E20"/>
       <c r="F20" t="n" s="2">
-        <v>43325.42435743056</v>
+        <v>43328.66248954861</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H20" t="s">
         <v>83</v>
@@ -1092,10 +1092,10 @@
         <v>83</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -1113,22 +1113,22 @@
       </c>
       <c r="E21"/>
       <c r="F21" t="n" s="2">
-        <v>43325.42435761574</v>
+        <v>43328.6624897338</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
         <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
@@ -1146,10 +1146,10 @@
       </c>
       <c r="E22"/>
       <c r="F22" t="n" s="2">
-        <v>43325.42435797454</v>
+        <v>43328.662489918985</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H22" t="s">
         <v>89</v>
@@ -1158,10 +1158,10 @@
         <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
@@ -1175,11 +1175,11 @@
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23"/>
       <c r="F23" t="n" s="2">
-        <v>43325.424358159726</v>
+        <v>43328.66249009259</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -1188,13 +1188,13 @@
         <v>92</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="J23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
@@ -1208,26 +1208,26 @@
         <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E24"/>
       <c r="F24" t="n" s="2">
-        <v>43325.42435833333</v>
+        <v>43328.66249027778</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H24" t="s">
         <v>95</v>
       </c>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
@@ -1241,11 +1241,11 @@
         <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E25"/>
       <c r="F25" t="n" s="2">
-        <v>43325.424358703705</v>
+        <v>43328.662490462964</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -1254,13 +1254,13 @@
         <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
@@ -1274,26 +1274,26 @@
         <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E26"/>
       <c r="F26" t="n" s="2">
-        <v>43325.42435887732</v>
+        <v>43328.662490636576</v>
       </c>
       <c r="G26" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
         <v>101</v>
       </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="J26" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="K26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
@@ -1307,26 +1307,26 @@
         <v>103</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E27"/>
       <c r="F27" t="n" s="2">
-        <v>43325.4243590625</v>
+        <v>43328.66249082176</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H27" t="s">
         <v>104</v>
       </c>
       <c r="I27" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J27" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E28"/>
       <c r="F28" t="n" s="2">
-        <v>43325.4243594213</v>
+        <v>43328.66249082176</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
@@ -1353,13 +1353,13 @@
         <v>107</v>
       </c>
       <c r="I28" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="J28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29">
@@ -1377,22 +1377,22 @@
       </c>
       <c r="E29"/>
       <c r="F29" t="n" s="2">
-        <v>43325.424359606484</v>
+        <v>43328.66249099537</v>
       </c>
       <c r="G29" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
         <v>110</v>
       </c>
       <c r="I29" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="K29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
@@ -1410,22 +1410,22 @@
       </c>
       <c r="E30"/>
       <c r="F30" t="n" s="2">
-        <v>43325.42435996528</v>
+        <v>43328.662491180556</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
         <v>113</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="J30" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="K30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="E31"/>
       <c r="F31" t="n" s="2">
-        <v>43325.424360150464</v>
+        <v>43328.66249136574</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
@@ -1452,13 +1452,13 @@
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="J31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>